<commit_message>
Base menor com tags
</commit_message>
<xml_diff>
--- a/bases/base-menor-tratada.xlsx
+++ b/bases/base-menor-tratada.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q100"/>
+  <dimension ref="A1:R100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,11 @@
           <t>semana_analise</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -581,6 +586,11 @@
       <c r="Q2" t="n">
         <v>1</v>
       </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -643,6 +653,11 @@
       </c>
       <c r="Q3" t="n">
         <v>1</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -707,6 +722,11 @@
       <c r="Q4" t="n">
         <v>1</v>
       </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -770,6 +790,11 @@
       <c r="Q5" t="n">
         <v>1</v>
       </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -833,6 +858,11 @@
       <c r="Q6" t="n">
         <v>1</v>
       </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -896,6 +926,11 @@
       <c r="Q7" t="n">
         <v>1</v>
       </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -958,6 +993,11 @@
       </c>
       <c r="Q8" t="n">
         <v>1</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -1022,6 +1062,11 @@
       <c r="Q9" t="n">
         <v>1</v>
       </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1085,6 +1130,11 @@
       <c r="Q10" t="n">
         <v>1</v>
       </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1148,6 +1198,11 @@
       <c r="Q11" t="n">
         <v>1</v>
       </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1211,6 +1266,11 @@
       <c r="Q12" t="n">
         <v>1</v>
       </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1274,6 +1334,11 @@
       <c r="Q13" t="n">
         <v>1</v>
       </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1337,6 +1402,11 @@
       <c r="Q14" t="n">
         <v>1</v>
       </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1400,6 +1470,11 @@
       <c r="Q15" t="n">
         <v>1</v>
       </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1463,6 +1538,11 @@
       <c r="Q16" t="n">
         <v>1</v>
       </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1526,6 +1606,11 @@
       <c r="Q17" t="n">
         <v>1</v>
       </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1589,6 +1674,11 @@
       <c r="Q18" t="n">
         <v>1</v>
       </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1652,6 +1742,11 @@
       <c r="Q19" t="n">
         <v>1</v>
       </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1715,6 +1810,11 @@
       <c r="Q20" t="n">
         <v>1</v>
       </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1778,6 +1878,11 @@
       <c r="Q21" t="n">
         <v>1</v>
       </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1841,6 +1946,11 @@
       <c r="Q22" t="n">
         <v>1</v>
       </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1904,6 +2014,11 @@
       <c r="Q23" t="n">
         <v>1</v>
       </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1967,6 +2082,11 @@
       <c r="Q24" t="n">
         <v>1</v>
       </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2029,6 +2149,11 @@
       </c>
       <c r="Q25" t="n">
         <v>1</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -2093,6 +2218,11 @@
       <c r="Q26" t="n">
         <v>1</v>
       </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2156,6 +2286,11 @@
       <c r="Q27" t="n">
         <v>1</v>
       </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2219,6 +2354,11 @@
       <c r="Q28" t="n">
         <v>1</v>
       </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2282,6 +2422,11 @@
       <c r="Q29" t="n">
         <v>1</v>
       </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2345,6 +2490,11 @@
       <c r="Q30" t="n">
         <v>1</v>
       </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2408,6 +2558,11 @@
       <c r="Q31" t="n">
         <v>1</v>
       </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2471,6 +2626,11 @@
       <c r="Q32" t="n">
         <v>1</v>
       </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2534,6 +2694,11 @@
       <c r="Q33" t="n">
         <v>1</v>
       </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2597,6 +2762,11 @@
       <c r="Q34" t="n">
         <v>1</v>
       </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2660,6 +2830,11 @@
       <c r="Q35" t="n">
         <v>1</v>
       </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2723,6 +2898,11 @@
       <c r="Q36" t="n">
         <v>1</v>
       </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2786,6 +2966,11 @@
       <c r="Q37" t="n">
         <v>1</v>
       </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2849,6 +3034,11 @@
       <c r="Q38" t="n">
         <v>1</v>
       </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2912,6 +3102,11 @@
       <c r="Q39" t="n">
         <v>1</v>
       </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2975,6 +3170,11 @@
       <c r="Q40" t="n">
         <v>1</v>
       </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3038,6 +3238,11 @@
       <c r="Q41" t="n">
         <v>1</v>
       </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3101,6 +3306,11 @@
       <c r="Q42" t="n">
         <v>1</v>
       </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3164,6 +3374,11 @@
       <c r="Q43" t="n">
         <v>1</v>
       </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -3227,6 +3442,11 @@
       <c r="Q44" t="n">
         <v>1</v>
       </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -3290,6 +3510,11 @@
       <c r="Q45" t="n">
         <v>1</v>
       </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -3353,6 +3578,11 @@
       <c r="Q46" t="n">
         <v>1</v>
       </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -3416,6 +3646,11 @@
       <c r="Q47" t="n">
         <v>1</v>
       </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -3479,6 +3714,11 @@
       <c r="Q48" t="n">
         <v>1</v>
       </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -3542,6 +3782,11 @@
       <c r="Q49" t="n">
         <v>1</v>
       </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -3605,6 +3850,11 @@
       <c r="Q50" t="n">
         <v>1</v>
       </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -3668,6 +3918,11 @@
       <c r="Q51" t="n">
         <v>1</v>
       </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -3731,6 +3986,11 @@
       <c r="Q52" t="n">
         <v>1</v>
       </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -3794,6 +4054,11 @@
       <c r="Q53" t="n">
         <v>1</v>
       </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3857,6 +4122,11 @@
       <c r="Q54" t="n">
         <v>1</v>
       </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -3920,6 +4190,11 @@
       <c r="Q55" t="n">
         <v>1</v>
       </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -3983,6 +4258,11 @@
       <c r="Q56" t="n">
         <v>1</v>
       </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -4046,6 +4326,11 @@
       <c r="Q57" t="n">
         <v>1</v>
       </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -4109,6 +4394,11 @@
       <c r="Q58" t="n">
         <v>1</v>
       </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -4172,6 +4462,11 @@
       <c r="Q59" t="n">
         <v>1</v>
       </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -4235,6 +4530,11 @@
       <c r="Q60" t="n">
         <v>1</v>
       </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -4298,6 +4598,11 @@
       <c r="Q61" t="n">
         <v>1</v>
       </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -4361,6 +4666,11 @@
       <c r="Q62" t="n">
         <v>1</v>
       </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -4424,6 +4734,11 @@
       <c r="Q63" t="n">
         <v>1</v>
       </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -4487,6 +4802,11 @@
       <c r="Q64" t="n">
         <v>1</v>
       </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -4550,6 +4870,11 @@
       <c r="Q65" t="n">
         <v>1</v>
       </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -4613,6 +4938,11 @@
       <c r="Q66" t="n">
         <v>1</v>
       </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -4676,6 +5006,11 @@
       <c r="Q67" t="n">
         <v>1</v>
       </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -4739,6 +5074,11 @@
       <c r="Q68" t="n">
         <v>1</v>
       </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -4802,6 +5142,11 @@
       <c r="Q69" t="n">
         <v>1</v>
       </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -4865,6 +5210,11 @@
       <c r="Q70" t="n">
         <v>1</v>
       </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -4928,6 +5278,11 @@
       <c r="Q71" t="n">
         <v>1</v>
       </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -4991,6 +5346,11 @@
       <c r="Q72" t="n">
         <v>1</v>
       </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -5054,6 +5414,11 @@
       <c r="Q73" t="n">
         <v>1</v>
       </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -5117,6 +5482,11 @@
       <c r="Q74" t="n">
         <v>1</v>
       </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -5180,6 +5550,11 @@
       <c r="Q75" t="n">
         <v>1</v>
       </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -5243,6 +5618,11 @@
       <c r="Q76" t="n">
         <v>1</v>
       </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -5306,6 +5686,11 @@
       <c r="Q77" t="n">
         <v>1</v>
       </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -5369,6 +5754,11 @@
       <c r="Q78" t="n">
         <v>1</v>
       </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -5432,6 +5822,11 @@
       <c r="Q79" t="n">
         <v>1</v>
       </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>['Lula', 'Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -5495,6 +5890,11 @@
       <c r="Q80" t="n">
         <v>1</v>
       </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -5558,6 +5958,11 @@
       <c r="Q81" t="n">
         <v>1</v>
       </c>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -5621,6 +6026,11 @@
       <c r="Q82" t="n">
         <v>1</v>
       </c>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -5684,6 +6094,11 @@
       <c r="Q83" t="n">
         <v>1</v>
       </c>
+      <c r="R83" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -5747,6 +6162,11 @@
       <c r="Q84" t="n">
         <v>1</v>
       </c>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -5810,6 +6230,11 @@
       <c r="Q85" t="n">
         <v>1</v>
       </c>
+      <c r="R85" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -5873,6 +6298,11 @@
       <c r="Q86" t="n">
         <v>1</v>
       </c>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -5936,6 +6366,11 @@
       <c r="Q87" t="n">
         <v>1</v>
       </c>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -5999,6 +6434,11 @@
       <c r="Q88" t="n">
         <v>1</v>
       </c>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -6062,6 +6502,11 @@
       <c r="Q89" t="n">
         <v>1</v>
       </c>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -6125,6 +6570,11 @@
       <c r="Q90" t="n">
         <v>1</v>
       </c>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -6188,6 +6638,11 @@
       <c r="Q91" t="n">
         <v>1</v>
       </c>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -6251,6 +6706,11 @@
       <c r="Q92" t="n">
         <v>1</v>
       </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -6314,6 +6774,11 @@
       <c r="Q93" t="n">
         <v>1</v>
       </c>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -6377,6 +6842,11 @@
       <c r="Q94" t="n">
         <v>1</v>
       </c>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>['Bolsonaro']</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -6440,6 +6910,11 @@
       <c r="Q95" t="n">
         <v>1</v>
       </c>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -6503,6 +6978,11 @@
       <c r="Q96" t="n">
         <v>1</v>
       </c>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -6566,6 +7046,11 @@
       <c r="Q97" t="n">
         <v>1</v>
       </c>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -6629,6 +7114,11 @@
       <c r="Q98" t="n">
         <v>1</v>
       </c>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -6692,6 +7182,11 @@
       <c r="Q99" t="n">
         <v>1</v>
       </c>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>['Lula']</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -6754,6 +7249,11 @@
       </c>
       <c r="Q100" t="n">
         <v>1</v>
+      </c>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação de coluna especifica para a citação de cada candidato
</commit_message>
<xml_diff>
--- a/bases/base-menor-tratada.xlsx
+++ b/bases/base-menor-tratada.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R100"/>
+  <dimension ref="A1:AA100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,52 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>lula</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>bolsonaro</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>ciro</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>simone_tebet</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>eymael</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>sofia_manzano</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>soraya_thronicke</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>felipe_d_avila</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>vera_lucia</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>leo_pericles</t>
         </is>
       </c>
     </row>
@@ -586,10 +631,35 @@
       <c r="Q2" t="n">
         <v>1</v>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -654,10 +724,35 @@
       <c r="Q3" t="n">
         <v>1</v>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -722,10 +817,35 @@
       <c r="Q4" t="n">
         <v>1</v>
       </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -790,10 +910,35 @@
       <c r="Q5" t="n">
         <v>1</v>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -858,10 +1003,35 @@
       <c r="Q6" t="n">
         <v>1</v>
       </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R6" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -926,10 +1096,35 @@
       <c r="Q7" t="n">
         <v>1</v>
       </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -994,10 +1189,35 @@
       <c r="Q8" t="n">
         <v>1</v>
       </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R8" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1062,10 +1282,35 @@
       <c r="Q9" t="n">
         <v>1</v>
       </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R9" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1130,10 +1375,35 @@
       <c r="Q10" t="n">
         <v>1</v>
       </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1198,10 +1468,35 @@
       <c r="Q11" t="n">
         <v>1</v>
       </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R11" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1266,10 +1561,35 @@
       <c r="Q12" t="n">
         <v>1</v>
       </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R12" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1334,10 +1654,35 @@
       <c r="Q13" t="n">
         <v>1</v>
       </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R13" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1402,10 +1747,35 @@
       <c r="Q14" t="n">
         <v>1</v>
       </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R14" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1470,10 +1840,35 @@
       <c r="Q15" t="n">
         <v>1</v>
       </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R15" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1538,10 +1933,35 @@
       <c r="Q16" t="n">
         <v>1</v>
       </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R16" t="n">
+        <v>1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1606,10 +2026,35 @@
       <c r="Q17" t="n">
         <v>1</v>
       </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R17" t="n">
+        <v>1</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1674,10 +2119,35 @@
       <c r="Q18" t="n">
         <v>1</v>
       </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R18" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1742,10 +2212,35 @@
       <c r="Q19" t="n">
         <v>1</v>
       </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1810,10 +2305,35 @@
       <c r="Q20" t="n">
         <v>1</v>
       </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R20" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1878,10 +2398,35 @@
       <c r="Q21" t="n">
         <v>1</v>
       </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R21" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1946,10 +2491,35 @@
       <c r="Q22" t="n">
         <v>1</v>
       </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R22" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2014,10 +2584,35 @@
       <c r="Q23" t="n">
         <v>1</v>
       </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R23" t="n">
+        <v>1</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2082,10 +2677,35 @@
       <c r="Q24" t="n">
         <v>1</v>
       </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R24" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2150,10 +2770,35 @@
       <c r="Q25" t="n">
         <v>1</v>
       </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R25" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2218,10 +2863,35 @@
       <c r="Q26" t="n">
         <v>1</v>
       </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R26" t="n">
+        <v>1</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -2286,10 +2956,35 @@
       <c r="Q27" t="n">
         <v>1</v>
       </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R27" t="n">
+        <v>1</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -2354,10 +3049,35 @@
       <c r="Q28" t="n">
         <v>1</v>
       </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R28" t="n">
+        <v>1</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2422,10 +3142,35 @@
       <c r="Q29" t="n">
         <v>1</v>
       </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R29" t="n">
+        <v>1</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2490,10 +3235,35 @@
       <c r="Q30" t="n">
         <v>1</v>
       </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R30" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2558,10 +3328,35 @@
       <c r="Q31" t="n">
         <v>1</v>
       </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R31" t="n">
+        <v>1</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2626,10 +3421,35 @@
       <c r="Q32" t="n">
         <v>1</v>
       </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>1</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2694,10 +3514,35 @@
       <c r="Q33" t="n">
         <v>1</v>
       </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>1</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2762,10 +3607,35 @@
       <c r="Q34" t="n">
         <v>1</v>
       </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>1</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2830,10 +3700,35 @@
       <c r="Q35" t="n">
         <v>1</v>
       </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>1</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2898,10 +3793,35 @@
       <c r="Q36" t="n">
         <v>1</v>
       </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="n">
+        <v>1</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2966,10 +3886,35 @@
       <c r="Q37" t="n">
         <v>1</v>
       </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3034,10 +3979,35 @@
       <c r="Q38" t="n">
         <v>1</v>
       </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>1</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -3102,10 +4072,35 @@
       <c r="Q39" t="n">
         <v>1</v>
       </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R39" t="n">
+        <v>1</v>
+      </c>
+      <c r="S39" t="n">
+        <v>1</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" t="n">
+        <v>0</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -3170,10 +4165,35 @@
       <c r="Q40" t="n">
         <v>1</v>
       </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="n">
+        <v>1</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="n">
+        <v>0</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -3238,10 +4258,35 @@
       <c r="Q41" t="n">
         <v>1</v>
       </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="n">
+        <v>0</v>
+      </c>
+      <c r="X41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -3306,10 +4351,35 @@
       <c r="Q42" t="n">
         <v>1</v>
       </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="n">
+        <v>1</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="n">
+        <v>0</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -3374,10 +4444,35 @@
       <c r="Q43" t="n">
         <v>1</v>
       </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="n">
+        <v>1</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" t="n">
+        <v>0</v>
+      </c>
+      <c r="W43" t="n">
+        <v>0</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -3442,10 +4537,35 @@
       <c r="Q44" t="n">
         <v>1</v>
       </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R44" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" t="n">
+        <v>1</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" t="n">
+        <v>0</v>
+      </c>
+      <c r="X44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -3510,10 +4630,35 @@
       <c r="Q45" t="n">
         <v>1</v>
       </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" t="n">
+        <v>1</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0</v>
+      </c>
+      <c r="W45" t="n">
+        <v>0</v>
+      </c>
+      <c r="X45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -3578,10 +4723,35 @@
       <c r="Q46" t="n">
         <v>1</v>
       </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="n">
+        <v>1</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0</v>
+      </c>
+      <c r="W46" t="n">
+        <v>0</v>
+      </c>
+      <c r="X46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -3646,10 +4816,35 @@
       <c r="Q47" t="n">
         <v>1</v>
       </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>1</v>
+      </c>
+      <c r="T47" t="n">
+        <v>0</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" t="n">
+        <v>0</v>
+      </c>
+      <c r="X47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -3714,10 +4909,35 @@
       <c r="Q48" t="n">
         <v>1</v>
       </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="n">
+        <v>1</v>
+      </c>
+      <c r="T48" t="n">
+        <v>0</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0</v>
+      </c>
+      <c r="V48" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" t="n">
+        <v>0</v>
+      </c>
+      <c r="X48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -3782,10 +5002,35 @@
       <c r="Q49" t="n">
         <v>1</v>
       </c>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R49" t="n">
+        <v>1</v>
+      </c>
+      <c r="S49" t="n">
+        <v>1</v>
+      </c>
+      <c r="T49" t="n">
+        <v>0</v>
+      </c>
+      <c r="U49" t="n">
+        <v>0</v>
+      </c>
+      <c r="V49" t="n">
+        <v>0</v>
+      </c>
+      <c r="W49" t="n">
+        <v>0</v>
+      </c>
+      <c r="X49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -3850,10 +5095,35 @@
       <c r="Q50" t="n">
         <v>1</v>
       </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>1</v>
+      </c>
+      <c r="T50" t="n">
+        <v>0</v>
+      </c>
+      <c r="U50" t="n">
+        <v>0</v>
+      </c>
+      <c r="V50" t="n">
+        <v>0</v>
+      </c>
+      <c r="W50" t="n">
+        <v>0</v>
+      </c>
+      <c r="X50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -3918,10 +5188,35 @@
       <c r="Q51" t="n">
         <v>1</v>
       </c>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="n">
+        <v>1</v>
+      </c>
+      <c r="T51" t="n">
+        <v>0</v>
+      </c>
+      <c r="U51" t="n">
+        <v>0</v>
+      </c>
+      <c r="V51" t="n">
+        <v>0</v>
+      </c>
+      <c r="W51" t="n">
+        <v>0</v>
+      </c>
+      <c r="X51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -3986,10 +5281,35 @@
       <c r="Q52" t="n">
         <v>1</v>
       </c>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="n">
+        <v>1</v>
+      </c>
+      <c r="T52" t="n">
+        <v>0</v>
+      </c>
+      <c r="U52" t="n">
+        <v>0</v>
+      </c>
+      <c r="V52" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" t="n">
+        <v>0</v>
+      </c>
+      <c r="X52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -4054,10 +5374,35 @@
       <c r="Q53" t="n">
         <v>1</v>
       </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="n">
+        <v>1</v>
+      </c>
+      <c r="T53" t="n">
+        <v>0</v>
+      </c>
+      <c r="U53" t="n">
+        <v>0</v>
+      </c>
+      <c r="V53" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" t="n">
+        <v>0</v>
+      </c>
+      <c r="X53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -4122,10 +5467,35 @@
       <c r="Q54" t="n">
         <v>1</v>
       </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R54" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="n">
+        <v>1</v>
+      </c>
+      <c r="T54" t="n">
+        <v>0</v>
+      </c>
+      <c r="U54" t="n">
+        <v>0</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0</v>
+      </c>
+      <c r="W54" t="n">
+        <v>0</v>
+      </c>
+      <c r="X54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -4190,10 +5560,35 @@
       <c r="Q55" t="n">
         <v>1</v>
       </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R55" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="n">
+        <v>1</v>
+      </c>
+      <c r="T55" t="n">
+        <v>0</v>
+      </c>
+      <c r="U55" t="n">
+        <v>0</v>
+      </c>
+      <c r="V55" t="n">
+        <v>0</v>
+      </c>
+      <c r="W55" t="n">
+        <v>0</v>
+      </c>
+      <c r="X55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -4258,10 +5653,35 @@
       <c r="Q56" t="n">
         <v>1</v>
       </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R56" t="n">
+        <v>0</v>
+      </c>
+      <c r="S56" t="n">
+        <v>1</v>
+      </c>
+      <c r="T56" t="n">
+        <v>0</v>
+      </c>
+      <c r="U56" t="n">
+        <v>0</v>
+      </c>
+      <c r="V56" t="n">
+        <v>0</v>
+      </c>
+      <c r="W56" t="n">
+        <v>0</v>
+      </c>
+      <c r="X56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -4326,10 +5746,35 @@
       <c r="Q57" t="n">
         <v>1</v>
       </c>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R57" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" t="n">
+        <v>1</v>
+      </c>
+      <c r="T57" t="n">
+        <v>0</v>
+      </c>
+      <c r="U57" t="n">
+        <v>0</v>
+      </c>
+      <c r="V57" t="n">
+        <v>0</v>
+      </c>
+      <c r="W57" t="n">
+        <v>0</v>
+      </c>
+      <c r="X57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -4394,10 +5839,35 @@
       <c r="Q58" t="n">
         <v>1</v>
       </c>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="n">
+        <v>1</v>
+      </c>
+      <c r="T58" t="n">
+        <v>0</v>
+      </c>
+      <c r="U58" t="n">
+        <v>0</v>
+      </c>
+      <c r="V58" t="n">
+        <v>0</v>
+      </c>
+      <c r="W58" t="n">
+        <v>0</v>
+      </c>
+      <c r="X58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -4462,10 +5932,35 @@
       <c r="Q59" t="n">
         <v>1</v>
       </c>
-      <c r="R59" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R59" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="n">
+        <v>1</v>
+      </c>
+      <c r="T59" t="n">
+        <v>0</v>
+      </c>
+      <c r="U59" t="n">
+        <v>0</v>
+      </c>
+      <c r="V59" t="n">
+        <v>0</v>
+      </c>
+      <c r="W59" t="n">
+        <v>0</v>
+      </c>
+      <c r="X59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -4530,10 +6025,35 @@
       <c r="Q60" t="n">
         <v>1</v>
       </c>
-      <c r="R60" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R60" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="n">
+        <v>1</v>
+      </c>
+      <c r="T60" t="n">
+        <v>0</v>
+      </c>
+      <c r="U60" t="n">
+        <v>0</v>
+      </c>
+      <c r="V60" t="n">
+        <v>0</v>
+      </c>
+      <c r="W60" t="n">
+        <v>0</v>
+      </c>
+      <c r="X60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -4598,10 +6118,35 @@
       <c r="Q61" t="n">
         <v>1</v>
       </c>
-      <c r="R61" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R61" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="n">
+        <v>0</v>
+      </c>
+      <c r="T61" t="n">
+        <v>0</v>
+      </c>
+      <c r="U61" t="n">
+        <v>0</v>
+      </c>
+      <c r="V61" t="n">
+        <v>0</v>
+      </c>
+      <c r="W61" t="n">
+        <v>0</v>
+      </c>
+      <c r="X61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -4666,10 +6211,35 @@
       <c r="Q62" t="n">
         <v>1</v>
       </c>
-      <c r="R62" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R62" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="n">
+        <v>1</v>
+      </c>
+      <c r="T62" t="n">
+        <v>1</v>
+      </c>
+      <c r="U62" t="n">
+        <v>0</v>
+      </c>
+      <c r="V62" t="n">
+        <v>0</v>
+      </c>
+      <c r="W62" t="n">
+        <v>0</v>
+      </c>
+      <c r="X62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -4734,10 +6304,35 @@
       <c r="Q63" t="n">
         <v>1</v>
       </c>
-      <c r="R63" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R63" t="n">
+        <v>0</v>
+      </c>
+      <c r="S63" t="n">
+        <v>0</v>
+      </c>
+      <c r="T63" t="n">
+        <v>1</v>
+      </c>
+      <c r="U63" t="n">
+        <v>0</v>
+      </c>
+      <c r="V63" t="n">
+        <v>0</v>
+      </c>
+      <c r="W63" t="n">
+        <v>0</v>
+      </c>
+      <c r="X63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -4802,10 +6397,35 @@
       <c r="Q64" t="n">
         <v>1</v>
       </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R64" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T64" t="n">
+        <v>1</v>
+      </c>
+      <c r="U64" t="n">
+        <v>0</v>
+      </c>
+      <c r="V64" t="n">
+        <v>0</v>
+      </c>
+      <c r="W64" t="n">
+        <v>0</v>
+      </c>
+      <c r="X64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -4870,10 +6490,35 @@
       <c r="Q65" t="n">
         <v>1</v>
       </c>
-      <c r="R65" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R65" t="n">
+        <v>0</v>
+      </c>
+      <c r="S65" t="n">
+        <v>0</v>
+      </c>
+      <c r="T65" t="n">
+        <v>1</v>
+      </c>
+      <c r="U65" t="n">
+        <v>0</v>
+      </c>
+      <c r="V65" t="n">
+        <v>0</v>
+      </c>
+      <c r="W65" t="n">
+        <v>0</v>
+      </c>
+      <c r="X65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -4938,10 +6583,35 @@
       <c r="Q66" t="n">
         <v>1</v>
       </c>
-      <c r="R66" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R66" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" t="n">
+        <v>1</v>
+      </c>
+      <c r="U66" t="n">
+        <v>0</v>
+      </c>
+      <c r="V66" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" t="n">
+        <v>0</v>
+      </c>
+      <c r="X66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -5006,10 +6676,35 @@
       <c r="Q67" t="n">
         <v>1</v>
       </c>
-      <c r="R67" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R67" t="n">
+        <v>0</v>
+      </c>
+      <c r="S67" t="n">
+        <v>0</v>
+      </c>
+      <c r="T67" t="n">
+        <v>1</v>
+      </c>
+      <c r="U67" t="n">
+        <v>0</v>
+      </c>
+      <c r="V67" t="n">
+        <v>0</v>
+      </c>
+      <c r="W67" t="n">
+        <v>0</v>
+      </c>
+      <c r="X67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -5074,10 +6769,35 @@
       <c r="Q68" t="n">
         <v>1</v>
       </c>
-      <c r="R68" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R68" t="n">
+        <v>1</v>
+      </c>
+      <c r="S68" t="n">
+        <v>0</v>
+      </c>
+      <c r="T68" t="n">
+        <v>1</v>
+      </c>
+      <c r="U68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V68" t="n">
+        <v>0</v>
+      </c>
+      <c r="W68" t="n">
+        <v>0</v>
+      </c>
+      <c r="X68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -5142,10 +6862,35 @@
       <c r="Q69" t="n">
         <v>1</v>
       </c>
-      <c r="R69" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R69" t="n">
+        <v>0</v>
+      </c>
+      <c r="S69" t="n">
+        <v>0</v>
+      </c>
+      <c r="T69" t="n">
+        <v>1</v>
+      </c>
+      <c r="U69" t="n">
+        <v>0</v>
+      </c>
+      <c r="V69" t="n">
+        <v>0</v>
+      </c>
+      <c r="W69" t="n">
+        <v>0</v>
+      </c>
+      <c r="X69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -5210,10 +6955,35 @@
       <c r="Q70" t="n">
         <v>1</v>
       </c>
-      <c r="R70" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R70" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="n">
+        <v>0</v>
+      </c>
+      <c r="T70" t="n">
+        <v>1</v>
+      </c>
+      <c r="U70" t="n">
+        <v>0</v>
+      </c>
+      <c r="V70" t="n">
+        <v>0</v>
+      </c>
+      <c r="W70" t="n">
+        <v>0</v>
+      </c>
+      <c r="X70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -5278,10 +7048,35 @@
       <c r="Q71" t="n">
         <v>1</v>
       </c>
-      <c r="R71" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R71" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" t="n">
+        <v>0</v>
+      </c>
+      <c r="T71" t="n">
+        <v>1</v>
+      </c>
+      <c r="U71" t="n">
+        <v>0</v>
+      </c>
+      <c r="V71" t="n">
+        <v>0</v>
+      </c>
+      <c r="W71" t="n">
+        <v>0</v>
+      </c>
+      <c r="X71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -5346,10 +7141,35 @@
       <c r="Q72" t="n">
         <v>1</v>
       </c>
-      <c r="R72" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R72" t="n">
+        <v>0</v>
+      </c>
+      <c r="S72" t="n">
+        <v>0</v>
+      </c>
+      <c r="T72" t="n">
+        <v>1</v>
+      </c>
+      <c r="U72" t="n">
+        <v>0</v>
+      </c>
+      <c r="V72" t="n">
+        <v>0</v>
+      </c>
+      <c r="W72" t="n">
+        <v>0</v>
+      </c>
+      <c r="X72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -5414,10 +7234,35 @@
       <c r="Q73" t="n">
         <v>1</v>
       </c>
-      <c r="R73" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R73" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="n">
+        <v>0</v>
+      </c>
+      <c r="T73" t="n">
+        <v>1</v>
+      </c>
+      <c r="U73" t="n">
+        <v>0</v>
+      </c>
+      <c r="V73" t="n">
+        <v>0</v>
+      </c>
+      <c r="W73" t="n">
+        <v>0</v>
+      </c>
+      <c r="X73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -5482,10 +7327,35 @@
       <c r="Q74" t="n">
         <v>1</v>
       </c>
-      <c r="R74" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R74" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="n">
+        <v>0</v>
+      </c>
+      <c r="T74" t="n">
+        <v>1</v>
+      </c>
+      <c r="U74" t="n">
+        <v>0</v>
+      </c>
+      <c r="V74" t="n">
+        <v>0</v>
+      </c>
+      <c r="W74" t="n">
+        <v>0</v>
+      </c>
+      <c r="X74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -5550,10 +7420,35 @@
       <c r="Q75" t="n">
         <v>1</v>
       </c>
-      <c r="R75" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R75" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="n">
+        <v>0</v>
+      </c>
+      <c r="T75" t="n">
+        <v>1</v>
+      </c>
+      <c r="U75" t="n">
+        <v>0</v>
+      </c>
+      <c r="V75" t="n">
+        <v>0</v>
+      </c>
+      <c r="W75" t="n">
+        <v>0</v>
+      </c>
+      <c r="X75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -5618,10 +7513,35 @@
       <c r="Q76" t="n">
         <v>1</v>
       </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R76" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" t="n">
+        <v>0</v>
+      </c>
+      <c r="T76" t="n">
+        <v>1</v>
+      </c>
+      <c r="U76" t="n">
+        <v>0</v>
+      </c>
+      <c r="V76" t="n">
+        <v>0</v>
+      </c>
+      <c r="W76" t="n">
+        <v>0</v>
+      </c>
+      <c r="X76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -5686,10 +7606,35 @@
       <c r="Q77" t="n">
         <v>1</v>
       </c>
-      <c r="R77" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R77" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" t="n">
+        <v>1</v>
+      </c>
+      <c r="T77" t="n">
+        <v>1</v>
+      </c>
+      <c r="U77" t="n">
+        <v>0</v>
+      </c>
+      <c r="V77" t="n">
+        <v>0</v>
+      </c>
+      <c r="W77" t="n">
+        <v>0</v>
+      </c>
+      <c r="X77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -5754,10 +7699,35 @@
       <c r="Q78" t="n">
         <v>1</v>
       </c>
-      <c r="R78" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R78" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" t="n">
+        <v>0</v>
+      </c>
+      <c r="T78" t="n">
+        <v>1</v>
+      </c>
+      <c r="U78" t="n">
+        <v>0</v>
+      </c>
+      <c r="V78" t="n">
+        <v>0</v>
+      </c>
+      <c r="W78" t="n">
+        <v>0</v>
+      </c>
+      <c r="X78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -5822,10 +7792,35 @@
       <c r="Q79" t="n">
         <v>1</v>
       </c>
-      <c r="R79" t="inlineStr">
-        <is>
-          <t>['Lula', 'Bolsonaro']</t>
-        </is>
+      <c r="R79" t="n">
+        <v>1</v>
+      </c>
+      <c r="S79" t="n">
+        <v>1</v>
+      </c>
+      <c r="T79" t="n">
+        <v>1</v>
+      </c>
+      <c r="U79" t="n">
+        <v>0</v>
+      </c>
+      <c r="V79" t="n">
+        <v>0</v>
+      </c>
+      <c r="W79" t="n">
+        <v>0</v>
+      </c>
+      <c r="X79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -5890,10 +7885,35 @@
       <c r="Q80" t="n">
         <v>1</v>
       </c>
-      <c r="R80" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R80" t="n">
+        <v>0</v>
+      </c>
+      <c r="S80" t="n">
+        <v>0</v>
+      </c>
+      <c r="T80" t="n">
+        <v>1</v>
+      </c>
+      <c r="U80" t="n">
+        <v>0</v>
+      </c>
+      <c r="V80" t="n">
+        <v>0</v>
+      </c>
+      <c r="W80" t="n">
+        <v>0</v>
+      </c>
+      <c r="X80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -5958,10 +7978,35 @@
       <c r="Q81" t="n">
         <v>1</v>
       </c>
-      <c r="R81" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R81" t="n">
+        <v>0</v>
+      </c>
+      <c r="S81" t="n">
+        <v>0</v>
+      </c>
+      <c r="T81" t="n">
+        <v>1</v>
+      </c>
+      <c r="U81" t="n">
+        <v>0</v>
+      </c>
+      <c r="V81" t="n">
+        <v>0</v>
+      </c>
+      <c r="W81" t="n">
+        <v>0</v>
+      </c>
+      <c r="X81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -6026,10 +8071,35 @@
       <c r="Q82" t="n">
         <v>1</v>
       </c>
-      <c r="R82" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R82" t="n">
+        <v>0</v>
+      </c>
+      <c r="S82" t="n">
+        <v>0</v>
+      </c>
+      <c r="T82" t="n">
+        <v>1</v>
+      </c>
+      <c r="U82" t="n">
+        <v>0</v>
+      </c>
+      <c r="V82" t="n">
+        <v>0</v>
+      </c>
+      <c r="W82" t="n">
+        <v>0</v>
+      </c>
+      <c r="X82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -6094,10 +8164,35 @@
       <c r="Q83" t="n">
         <v>1</v>
       </c>
-      <c r="R83" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R83" t="n">
+        <v>0</v>
+      </c>
+      <c r="S83" t="n">
+        <v>0</v>
+      </c>
+      <c r="T83" t="n">
+        <v>1</v>
+      </c>
+      <c r="U83" t="n">
+        <v>0</v>
+      </c>
+      <c r="V83" t="n">
+        <v>0</v>
+      </c>
+      <c r="W83" t="n">
+        <v>0</v>
+      </c>
+      <c r="X83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -6162,10 +8257,35 @@
       <c r="Q84" t="n">
         <v>1</v>
       </c>
-      <c r="R84" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R84" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="n">
+        <v>0</v>
+      </c>
+      <c r="T84" t="n">
+        <v>1</v>
+      </c>
+      <c r="U84" t="n">
+        <v>0</v>
+      </c>
+      <c r="V84" t="n">
+        <v>0</v>
+      </c>
+      <c r="W84" t="n">
+        <v>0</v>
+      </c>
+      <c r="X84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -6230,10 +8350,35 @@
       <c r="Q85" t="n">
         <v>1</v>
       </c>
-      <c r="R85" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R85" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T85" t="n">
+        <v>1</v>
+      </c>
+      <c r="U85" t="n">
+        <v>0</v>
+      </c>
+      <c r="V85" t="n">
+        <v>0</v>
+      </c>
+      <c r="W85" t="n">
+        <v>0</v>
+      </c>
+      <c r="X85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -6298,10 +8443,35 @@
       <c r="Q86" t="n">
         <v>1</v>
       </c>
-      <c r="R86" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R86" t="n">
+        <v>0</v>
+      </c>
+      <c r="S86" t="n">
+        <v>0</v>
+      </c>
+      <c r="T86" t="n">
+        <v>1</v>
+      </c>
+      <c r="U86" t="n">
+        <v>0</v>
+      </c>
+      <c r="V86" t="n">
+        <v>0</v>
+      </c>
+      <c r="W86" t="n">
+        <v>0</v>
+      </c>
+      <c r="X86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA86" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -6366,10 +8536,35 @@
       <c r="Q87" t="n">
         <v>1</v>
       </c>
-      <c r="R87" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R87" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="n">
+        <v>0</v>
+      </c>
+      <c r="T87" t="n">
+        <v>1</v>
+      </c>
+      <c r="U87" t="n">
+        <v>0</v>
+      </c>
+      <c r="V87" t="n">
+        <v>0</v>
+      </c>
+      <c r="W87" t="n">
+        <v>0</v>
+      </c>
+      <c r="X87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -6434,10 +8629,35 @@
       <c r="Q88" t="n">
         <v>1</v>
       </c>
-      <c r="R88" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R88" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="n">
+        <v>0</v>
+      </c>
+      <c r="T88" t="n">
+        <v>1</v>
+      </c>
+      <c r="U88" t="n">
+        <v>0</v>
+      </c>
+      <c r="V88" t="n">
+        <v>0</v>
+      </c>
+      <c r="W88" t="n">
+        <v>0</v>
+      </c>
+      <c r="X88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -6502,10 +8722,35 @@
       <c r="Q89" t="n">
         <v>1</v>
       </c>
-      <c r="R89" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R89" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" t="n">
+        <v>0</v>
+      </c>
+      <c r="T89" t="n">
+        <v>1</v>
+      </c>
+      <c r="U89" t="n">
+        <v>0</v>
+      </c>
+      <c r="V89" t="n">
+        <v>0</v>
+      </c>
+      <c r="W89" t="n">
+        <v>0</v>
+      </c>
+      <c r="X89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA89" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -6570,10 +8815,35 @@
       <c r="Q90" t="n">
         <v>1</v>
       </c>
-      <c r="R90" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R90" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="n">
+        <v>0</v>
+      </c>
+      <c r="T90" t="n">
+        <v>1</v>
+      </c>
+      <c r="U90" t="n">
+        <v>0</v>
+      </c>
+      <c r="V90" t="n">
+        <v>0</v>
+      </c>
+      <c r="W90" t="n">
+        <v>0</v>
+      </c>
+      <c r="X90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -6638,10 +8908,35 @@
       <c r="Q91" t="n">
         <v>1</v>
       </c>
-      <c r="R91" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R91" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="n">
+        <v>0</v>
+      </c>
+      <c r="T91" t="n">
+        <v>1</v>
+      </c>
+      <c r="U91" t="n">
+        <v>0</v>
+      </c>
+      <c r="V91" t="n">
+        <v>0</v>
+      </c>
+      <c r="W91" t="n">
+        <v>0</v>
+      </c>
+      <c r="X91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA91" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -6706,10 +9001,35 @@
       <c r="Q92" t="n">
         <v>1</v>
       </c>
-      <c r="R92" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R92" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="n">
+        <v>1</v>
+      </c>
+      <c r="V92" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="n">
+        <v>0</v>
+      </c>
+      <c r="X92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -6774,10 +9094,35 @@
       <c r="Q93" t="n">
         <v>1</v>
       </c>
-      <c r="R93" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R93" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="n">
+        <v>0</v>
+      </c>
+      <c r="T93" t="n">
+        <v>0</v>
+      </c>
+      <c r="U93" t="n">
+        <v>1</v>
+      </c>
+      <c r="V93" t="n">
+        <v>0</v>
+      </c>
+      <c r="W93" t="n">
+        <v>0</v>
+      </c>
+      <c r="X93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -6842,10 +9187,35 @@
       <c r="Q94" t="n">
         <v>1</v>
       </c>
-      <c r="R94" t="inlineStr">
-        <is>
-          <t>['Bolsonaro']</t>
-        </is>
+      <c r="R94" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="n">
+        <v>1</v>
+      </c>
+      <c r="T94" t="n">
+        <v>0</v>
+      </c>
+      <c r="U94" t="n">
+        <v>1</v>
+      </c>
+      <c r="V94" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" t="n">
+        <v>0</v>
+      </c>
+      <c r="X94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA94" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -6910,10 +9280,35 @@
       <c r="Q95" t="n">
         <v>1</v>
       </c>
-      <c r="R95" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R95" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="n">
+        <v>0</v>
+      </c>
+      <c r="T95" t="n">
+        <v>0</v>
+      </c>
+      <c r="U95" t="n">
+        <v>1</v>
+      </c>
+      <c r="V95" t="n">
+        <v>0</v>
+      </c>
+      <c r="W95" t="n">
+        <v>0</v>
+      </c>
+      <c r="X95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA95" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -6978,10 +9373,35 @@
       <c r="Q96" t="n">
         <v>1</v>
       </c>
-      <c r="R96" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R96" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" t="n">
+        <v>0</v>
+      </c>
+      <c r="T96" t="n">
+        <v>0</v>
+      </c>
+      <c r="U96" t="n">
+        <v>1</v>
+      </c>
+      <c r="V96" t="n">
+        <v>0</v>
+      </c>
+      <c r="W96" t="n">
+        <v>0</v>
+      </c>
+      <c r="X96" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y96" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -7046,10 +9466,35 @@
       <c r="Q97" t="n">
         <v>1</v>
       </c>
-      <c r="R97" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R97" t="n">
+        <v>0</v>
+      </c>
+      <c r="S97" t="n">
+        <v>0</v>
+      </c>
+      <c r="T97" t="n">
+        <v>0</v>
+      </c>
+      <c r="U97" t="n">
+        <v>1</v>
+      </c>
+      <c r="V97" t="n">
+        <v>0</v>
+      </c>
+      <c r="W97" t="n">
+        <v>0</v>
+      </c>
+      <c r="X97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA97" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -7114,10 +9559,35 @@
       <c r="Q98" t="n">
         <v>1</v>
       </c>
-      <c r="R98" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R98" t="n">
+        <v>1</v>
+      </c>
+      <c r="S98" t="n">
+        <v>0</v>
+      </c>
+      <c r="T98" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="n">
+        <v>1</v>
+      </c>
+      <c r="V98" t="n">
+        <v>0</v>
+      </c>
+      <c r="W98" t="n">
+        <v>0</v>
+      </c>
+      <c r="X98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA98" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -7182,10 +9652,35 @@
       <c r="Q99" t="n">
         <v>1</v>
       </c>
-      <c r="R99" t="inlineStr">
-        <is>
-          <t>['Lula']</t>
-        </is>
+      <c r="R99" t="n">
+        <v>1</v>
+      </c>
+      <c r="S99" t="n">
+        <v>0</v>
+      </c>
+      <c r="T99" t="n">
+        <v>1</v>
+      </c>
+      <c r="U99" t="n">
+        <v>1</v>
+      </c>
+      <c r="V99" t="n">
+        <v>0</v>
+      </c>
+      <c r="W99" t="n">
+        <v>0</v>
+      </c>
+      <c r="X99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA99" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -7250,10 +9745,35 @@
       <c r="Q100" t="n">
         <v>1</v>
       </c>
-      <c r="R100" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="R100" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" t="n">
+        <v>0</v>
+      </c>
+      <c r="T100" t="n">
+        <v>0</v>
+      </c>
+      <c r="U100" t="n">
+        <v>1</v>
+      </c>
+      <c r="V100" t="n">
+        <v>0</v>
+      </c>
+      <c r="W100" t="n">
+        <v>0</v>
+      </c>
+      <c r="X100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA100" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>